<commit_message>
Lo trabajado en clase el 21/10/2024
</commit_message>
<xml_diff>
--- a/ASIGNATURAS/HorarioClasesFP.xlsx
+++ b/ASIGNATURAS/HorarioClasesFP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CursoFP2\ASIGNATURAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44AC5BB-84CA-45C0-AA65-8189C014AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77DAD397-D190-49A9-9E71-B7E6F88F769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAB098BD-E893-422D-AFC5-FB3FDBA1881A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
   <si>
     <t>15:30-16:25</t>
   </si>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -199,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,13 +230,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -257,7 +302,46 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Énfasis5" xfId="2" builtinId="47"/>
@@ -582,19 +666,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A80F64-377D-449E-BA9F-A929F6EEF00F}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="6" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="14" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>4</v>
@@ -611,8 +697,24 @@
       <c r="F1" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -631,8 +733,26 @@
       <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -651,8 +771,16 @@
       <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="I3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="15"/>
     </row>
-    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -671,8 +799,26 @@
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="I4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -683,8 +829,18 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -694,18 +850,35 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>18</v>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="L6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -715,17 +888,33 @@
       <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -735,19 +924,41 @@
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="12">
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>